<commit_message>
Backup QR Scanner data - 2025-12-23T08:47:18.270Z - Cache Bust: 1766479638270
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1765109770507_f71267414ad928ff5abcafbc64a0ab66be7858c72295754f0460aad3fd95b393.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1765109770507_f71267414ad928ff5abcafbc64a0ab66be7858c72295754f0460aad3fd95b393.xlsx
@@ -439,7 +439,7 @@
         <v>Manual</v>
       </c>
       <c r="F2" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="3">
@@ -459,7 +459,7 @@
         <v>Manual</v>
       </c>
       <c r="F3" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="4">
@@ -479,7 +479,7 @@
         <v>Manual</v>
       </c>
       <c r="F4" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="5">
@@ -499,7 +499,7 @@
         <v>Manual</v>
       </c>
       <c r="F5" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="6">
@@ -519,7 +519,7 @@
         <v>Manual</v>
       </c>
       <c r="F6" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="7">
@@ -539,7 +539,7 @@
         <v>Manual</v>
       </c>
       <c r="F7" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="8">
@@ -559,7 +559,7 @@
         <v>Manual</v>
       </c>
       <c r="F8" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="9">
@@ -579,7 +579,7 @@
         <v>Manual</v>
       </c>
       <c r="F9" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="10">
@@ -599,7 +599,7 @@
         <v>Manual</v>
       </c>
       <c r="F10" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="11">
@@ -619,7 +619,7 @@
         <v>Manual</v>
       </c>
       <c r="F11" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="12">
@@ -639,7 +639,7 @@
         <v>Manual</v>
       </c>
       <c r="F12" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="13">
@@ -659,7 +659,7 @@
         <v>Manual</v>
       </c>
       <c r="F13" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="14">
@@ -679,7 +679,7 @@
         <v>Manual</v>
       </c>
       <c r="F14" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="15">
@@ -699,7 +699,7 @@
         <v>Manual</v>
       </c>
       <c r="F15" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="16">
@@ -719,7 +719,7 @@
         <v>Manual</v>
       </c>
       <c r="F16" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="17">
@@ -739,7 +739,7 @@
         <v>Manual</v>
       </c>
       <c r="F17" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="18">
@@ -759,7 +759,7 @@
         <v>Manual</v>
       </c>
       <c r="F18" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="19">
@@ -779,7 +779,7 @@
         <v>Manual</v>
       </c>
       <c r="F19" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="20">
@@ -799,7 +799,7 @@
         <v>Manual</v>
       </c>
       <c r="F20" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="21">
@@ -819,7 +819,7 @@
         <v>Manual</v>
       </c>
       <c r="F21" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="22">
@@ -839,7 +839,7 @@
         <v>Manual</v>
       </c>
       <c r="F22" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="23">
@@ -859,7 +859,7 @@
         <v>Manual</v>
       </c>
       <c r="F23" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="24">
@@ -879,7 +879,7 @@
         <v>Manual</v>
       </c>
       <c r="F24" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="25">
@@ -899,7 +899,7 @@
         <v>Manual</v>
       </c>
       <c r="F25" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="26">
@@ -919,7 +919,7 @@
         <v>Manual</v>
       </c>
       <c r="F26" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="27">
@@ -939,7 +939,7 @@
         <v>Manual</v>
       </c>
       <c r="F27" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="28">
@@ -959,7 +959,7 @@
         <v>Manual</v>
       </c>
       <c r="F28" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="29">
@@ -979,7 +979,7 @@
         <v>Manual</v>
       </c>
       <c r="F29" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="30">
@@ -999,7 +999,7 @@
         <v>Manual</v>
       </c>
       <c r="F30" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="31">
@@ -1019,7 +1019,7 @@
         <v>Manual</v>
       </c>
       <c r="F31" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="32">
@@ -1039,7 +1039,7 @@
         <v>Manual</v>
       </c>
       <c r="F32" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="33">
@@ -1059,7 +1059,7 @@
         <v>Manual</v>
       </c>
       <c r="F33" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="34">
@@ -1079,7 +1079,7 @@
         <v>Manual</v>
       </c>
       <c r="F34" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="35">
@@ -1099,7 +1099,7 @@
         <v>Manual</v>
       </c>
       <c r="F35" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="36">
@@ -1119,7 +1119,7 @@
         <v>Manual</v>
       </c>
       <c r="F36" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="37">
@@ -1139,7 +1139,7 @@
         <v>Manual</v>
       </c>
       <c r="F37" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="38">
@@ -1159,7 +1159,7 @@
         <v>Manual</v>
       </c>
       <c r="F38" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="39">
@@ -1179,7 +1179,7 @@
         <v>Manual</v>
       </c>
       <c r="F39" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="40">
@@ -1199,7 +1199,7 @@
         <v>Manual</v>
       </c>
       <c r="F40" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="41">
@@ -1219,7 +1219,7 @@
         <v>Manual</v>
       </c>
       <c r="F41" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="42">
@@ -1239,7 +1239,7 @@
         <v>Manual</v>
       </c>
       <c r="F42" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="43">
@@ -1259,7 +1259,7 @@
         <v>Manual</v>
       </c>
       <c r="F43" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
     <row r="44">
@@ -1279,7 +1279,7 @@
         <v>Manual</v>
       </c>
       <c r="F44" t="str">
-        <v>Emp16.farida.m.abdelaziz@gmail.com</v>
+        <v>emp16.farida.m.abdelaziz@gmail.com</v>
       </c>
     </row>
   </sheetData>

</xml_diff>